<commit_message>
first version of compatibility score calculations
</commit_message>
<xml_diff>
--- a/data/Matching_Template.xlsx
+++ b/data/Matching_Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csw066\OneDrive - Queen Mary, University of London\0001 QMentoring\06 Other Projects\Algorithm Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Admin/Desktop/MyDocs/QMentoring algo/Mentor-Matching-Algo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3090F6-62D9-8142-9B6C-381C1BBC2118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12060" tabRatio="599"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12060" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mentor data" sheetId="13" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="58">
   <si>
     <t>First Name:</t>
   </si>
@@ -191,12 +192,24 @@
   </si>
   <si>
     <t>N/A - example</t>
+  </si>
+  <si>
+    <t>Mentor1</t>
+  </si>
+  <si>
+    <t>Mentor2</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -570,40 +583,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="54.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="93.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="52.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="61.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="47.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.08984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="64.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="115.6328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.6328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="54.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="93.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="61.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="47.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="64.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="115.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="31" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="51.1796875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="255.6328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="141.08984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="51.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="255.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="141.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -671,12 +684,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>53</v>
@@ -735,46 +748,54 @@
         <v>21</v>
       </c>
     </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:V2"/>
+  <autoFilter ref="A1:V2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T68"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B39" sqref="B39:B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="12.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="52.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="78.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="52.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="78.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="50" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="77.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="115.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="115.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="166.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="37.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.7265625" style="2"/>
+    <col min="15" max="15" width="34.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="77.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="115.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="115.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="166.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="37.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -836,7 +857,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>53</v>
       </c>
@@ -883,23 +904,23 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="D3" s="10"/>
     </row>
-    <row r="4" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="D5" s="10"/>
     </row>
-    <row r="6" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -921,7 +942,7 @@
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
     </row>
-    <row r="8" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="10"/>
@@ -942,7 +963,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -964,31 +985,31 @@
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
     </row>
-    <row r="10" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1010,236 +1031,250 @@
       <c r="S16" s="6"/>
       <c r="T16" s="6"/>
     </row>
-    <row r="17" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="D17" s="10"/>
     </row>
-    <row r="18" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
       <c r="D26" s="10"/>
     </row>
-    <row r="27" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="D27" s="10"/>
     </row>
-    <row r="28" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="D29" s="10"/>
     </row>
-    <row r="30" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="C30" s="11"/>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="D31" s="10"/>
     </row>
-    <row r="32" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
       <c r="D32" s="10"/>
     </row>
-    <row r="33" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="D33" s="10"/>
     </row>
-    <row r="34" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
       <c r="D34" s="10"/>
     </row>
-    <row r="35" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="D35" s="10"/>
     </row>
-    <row r="36" spans="1:4" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6"/>
       <c r="D36" s="10"/>
     </row>
-    <row r="37" spans="1:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
       <c r="D37" s="10"/>
     </row>
-    <row r="38" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="6"/>
       <c r="C38" s="8"/>
       <c r="D38" s="10"/>
     </row>
-    <row r="39" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
       <c r="C39" s="8"/>
       <c r="D39" s="10"/>
     </row>
-    <row r="40" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="6"/>
       <c r="D40" s="10"/>
     </row>
-    <row r="41" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
       <c r="D41" s="10"/>
     </row>
-    <row r="42" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="6"/>
       <c r="D42" s="10"/>
     </row>
-    <row r="43" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="D43" s="10"/>
     </row>
-    <row r="44" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="6"/>
       <c r="D44" s="10"/>
     </row>
-    <row r="45" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
       <c r="D45" s="10"/>
     </row>
-    <row r="46" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="6"/>
       <c r="D46" s="10"/>
     </row>
-    <row r="47" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
       <c r="D47" s="10"/>
     </row>
-    <row r="48" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
       <c r="C48" s="8"/>
       <c r="D48" s="10"/>
     </row>
-    <row r="49" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
       <c r="C49" s="8"/>
       <c r="D49" s="10"/>
     </row>
-    <row r="50" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="6"/>
       <c r="D50" s="10"/>
     </row>
-    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
       <c r="D51" s="10"/>
     </row>
-    <row r="52" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="6"/>
       <c r="D52" s="10"/>
     </row>
-    <row r="53" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="6"/>
       <c r="D53" s="10"/>
     </row>
-    <row r="54" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="6"/>
       <c r="D54" s="10"/>
     </row>
-    <row r="55" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="6"/>
       <c r="D55" s="10"/>
     </row>
-    <row r="56" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="6"/>
       <c r="D56" s="10"/>
     </row>
-    <row r="57" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="6"/>
       <c r="D57" s="10"/>
     </row>
-    <row r="58" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="6"/>
       <c r="D58" s="10"/>
     </row>
-    <row r="59" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="6"/>
       <c r="D59" s="10"/>
     </row>
-    <row r="60" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="6"/>
       <c r="D60" s="10"/>
     </row>
-    <row r="61" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="6"/>
       <c r="C61" s="8"/>
       <c r="D61" s="10"/>
     </row>
-    <row r="62" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="6"/>
       <c r="D62" s="10"/>
     </row>
-    <row r="63" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="6"/>
       <c r="C63" s="6"/>
       <c r="D63" s="10"/>
     </row>
-    <row r="64" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="6"/>
       <c r="D64" s="10"/>
     </row>
-    <row r="65" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="6"/>
       <c r="D65" s="10"/>
     </row>
-    <row r="66" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="6"/>
       <c r="C66" s="8"/>
       <c r="D66" s="10"/>
     </row>
-    <row r="67" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="6"/>
       <c r="D67" s="10"/>
     </row>
-    <row r="68" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="6"/>
       <c r="D68" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T69"/>
+  <autoFilter ref="A1:T69" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="9c18f9b8-5ae4-4f0b-a238-a922c51e2dda" ContentTypeId="0x0101005EA864BF41DF8A41860E925F5B29BCF5" PreviousValue="false"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="45ae7f3d-bcd0-4e4b-af93-f03a9fbb19b5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010005654ADC9F12924A98775CE4A71E31EA" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="549651e92ced56e5a1de0cf17176f363">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="45ae7f3d-bcd0-4e4b-af93-f03a9fbb19b5" xmlns:ns3="6649982f-b66b-4072-8006-4697fed55f9d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="137a0823a5661f7a32d06da009f93573" ns2:_="" ns3:_="">
     <xsd:import namespace="45ae7f3d-bcd0-4e4b-af93-f03a9fbb19b5"/>
@@ -1470,46 +1505,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="45ae7f3d-bcd0-4e4b-af93-f03a9fbb19b5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56CEDA22-76A3-434D-90BB-587C84455EF5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF170D63-66F2-46E6-B806-90D03EC8C80C}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D8735D6-5637-44D0-BD2B-562E57FE7972}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F65F4A3-B4B1-492D-BDDD-4EE4941835A4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -1522,6 +1518,34 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="45ae7f3d-bcd0-4e4b-af93-f03a9fbb19b5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D8735D6-5637-44D0-BD2B-562E57FE7972}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF170D63-66F2-46E6-B806-90D03EC8C80C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="45ae7f3d-bcd0-4e4b-af93-f03a9fbb19b5"/>
+    <ds:schemaRef ds:uri="6649982f-b66b-4072-8006-4697fed55f9d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>